<commit_message>
Cambio nombre reporte de Auditoria
COLOCAR = REPORTE PRECIOS MATERIAS PRIMAS
</commit_message>
<xml_diff>
--- a/public/assets/plantillas_excel/Reporte_003A.xlsx
+++ b/public/assets/plantillas_excel/Reporte_003A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/htdocs/reporteador/public/assets/plantillas_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02E4FD1B-933A-4249-A314-62BD11FD72F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F18FBA5-3A21-2E42-829D-850CE8C01404}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,6 @@
     <t>No. 003-A</t>
   </si>
   <si>
-    <t>003-A AUDITORIA DE COSTOS</t>
-  </si>
-  <si>
     <t>CODIGO</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>U_COMPRA</t>
+  </si>
+  <si>
+    <t>003-A REPORTE PRECIOS MATERIAS PRIMAS.</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -455,7 +455,7 @@
     </row>
     <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -466,31 +466,31 @@
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>